<commit_message>
All working fine as per requirements given
</commit_message>
<xml_diff>
--- a/Wage Report_for All categories_GWC.xlsx
+++ b/Wage Report_for All categories_GWC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF56638-CF5D-41EF-9C99-9E95F906F19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D6349D-59FC-4BE2-B0B4-F94547BD7388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00FDC47E-B757-4224-8668-0EA62B941A79}"/>
   </bookViews>
@@ -13,6 +13,9 @@
     <sheet name="Job Descriptions" sheetId="2" r:id="rId3"/>
     <sheet name="Reliability by Job and Area" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Advanced Reports'!$B$1:$B$1106</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6716" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6713" uniqueCount="170">
   <si>
     <t xml:space="preserve">ERI's Global Salary Calculator </t>
   </si>
@@ -1371,10 +1374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F972A4-0392-43E1-9B90-6D4DECD827DB}">
-  <dimension ref="A1:M1113"/>
+  <dimension ref="A1:M1106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1087" workbookViewId="0">
+      <selection activeCell="B1109" sqref="B1109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51150,74 +51153,8 @@
         <v>6.7008545000000002</v>
       </c>
     </row>
-    <row r="1107" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1107" s="12"/>
-      <c r="B1107" s="12"/>
-      <c r="C1107" s="12"/>
-      <c r="D1107" s="12"/>
-      <c r="E1107" s="12"/>
-      <c r="F1107" s="12"/>
-      <c r="G1107" s="12"/>
-      <c r="H1107" s="12"/>
-      <c r="I1107" s="12"/>
-    </row>
-    <row r="1111" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1111" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1111" s="34"/>
-      <c r="C1111" s="34"/>
-      <c r="D1111" s="34"/>
-      <c r="E1111" s="34"/>
-      <c r="F1111" s="34"/>
-      <c r="G1111" s="34"/>
-      <c r="H1111" s="34"/>
-      <c r="I1111" s="34"/>
-      <c r="J1111" s="34"/>
-      <c r="K1111" s="34"/>
-      <c r="L1111" s="34"/>
-      <c r="M1111" s="34"/>
-    </row>
-    <row r="1112" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1112" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1112" s="34"/>
-      <c r="C1112" s="34"/>
-      <c r="D1112" s="34"/>
-      <c r="E1112" s="34"/>
-      <c r="F1112" s="34"/>
-      <c r="G1112" s="34"/>
-      <c r="H1112" s="34"/>
-      <c r="I1112" s="34"/>
-      <c r="J1112" s="34"/>
-      <c r="K1112" s="34"/>
-      <c r="L1112" s="34"/>
-      <c r="M1112" s="34"/>
-    </row>
-    <row r="1113" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1113" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1113" s="34"/>
-      <c r="C1113" s="34"/>
-      <c r="D1113" s="34"/>
-      <c r="E1113" s="34"/>
-      <c r="F1113" s="34"/>
-      <c r="G1113" s="34"/>
-      <c r="H1113" s="34"/>
-      <c r="I1113" s="34"/>
-      <c r="J1113" s="34"/>
-      <c r="K1113" s="34"/>
-      <c r="L1113" s="34"/>
-      <c r="M1113" s="34"/>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1111:M1111"/>
-    <mergeCell ref="A1112:M1112"/>
-    <mergeCell ref="A1113:M1113"/>
-  </mergeCells>
+  <autoFilter ref="B1:B1106" xr:uid="{09F972A4-0392-43E1-9B90-6D4DECD827DB}"/>
   <conditionalFormatting sqref="D2:H1106">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>ISNUMBER(SEARCH("Hourly",#REF!))</formula>

</xml_diff>